<commit_message>
Añadida visualización en tiempo real y guardado en SQLite
</commit_message>
<xml_diff>
--- a/datos_sensores_0001.xlsx
+++ b/datos_sensores_0001.xlsx
@@ -463,188 +463,188 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:02</t>
+          <t>2025-06-08 01:48:38</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>25.3</v>
+        <v>27.5</v>
       </c>
       <c r="C2" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D2" t="n">
-        <v>1010.85</v>
+        <v>1010.26</v>
       </c>
       <c r="E2" t="n">
-        <v>17.5</v>
+        <v>15.83</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:04</t>
+          <t>2025-06-08 01:48:40</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>25.3</v>
+        <v>27.1</v>
       </c>
       <c r="C3" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D3" t="n">
-        <v>1010.88</v>
+        <v>1010.27</v>
       </c>
       <c r="E3" t="n">
-        <v>17.5</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:06</t>
+          <t>2025-06-08 01:48:42</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25.3</v>
+        <v>27.1</v>
       </c>
       <c r="C4" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D4" t="n">
-        <v>1010.85</v>
+        <v>1010.26</v>
       </c>
       <c r="E4" t="n">
-        <v>20</v>
+        <v>18.33</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:09</t>
+          <t>2025-06-08 01:48:45</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25.3</v>
+        <v>27.1</v>
       </c>
       <c r="C5" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D5" t="n">
-        <v>1010.84</v>
+        <v>1010.28</v>
       </c>
       <c r="E5" t="n">
-        <v>20</v>
+        <v>19.17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:11</t>
+          <t>2025-06-08 01:48:47</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25.3</v>
+        <v>27.1</v>
       </c>
       <c r="C6" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D6" t="n">
-        <v>1010.85</v>
+        <v>1010.26</v>
       </c>
       <c r="E6" t="n">
-        <v>18.33</v>
+        <v>19.17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:13</t>
+          <t>2025-06-08 01:48:49</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>25.3</v>
+        <v>27.1</v>
       </c>
       <c r="C7" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D7" t="n">
-        <v>1010.83</v>
+        <v>1010.24</v>
       </c>
       <c r="E7" t="n">
-        <v>17.5</v>
+        <v>19.17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:15</t>
+          <t>2025-06-08 01:48:51</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>25.7</v>
+        <v>27.1</v>
       </c>
       <c r="C8" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D8" t="n">
-        <v>1010.8</v>
+        <v>1010.25</v>
       </c>
       <c r="E8" t="n">
-        <v>14.17</v>
+        <v>19.17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:17</t>
+          <t>2025-06-08 01:48:53</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>25.8</v>
+        <v>27.1</v>
       </c>
       <c r="C9" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D9" t="n">
-        <v>1010.87</v>
+        <v>1010.27</v>
       </c>
       <c r="E9" t="n">
-        <v>17.5</v>
+        <v>19.17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:19</t>
+          <t>2025-06-08 01:48:55</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>25.8</v>
+        <v>27.1</v>
       </c>
       <c r="C10" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D10" t="n">
-        <v>1010.9</v>
+        <v>1010.21</v>
       </c>
       <c r="E10" t="n">
-        <v>17.5</v>
+        <v>19.17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:21</t>
+          <t>2025-06-08 01:48:57</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>25.8</v>
+        <v>27.1</v>
       </c>
       <c r="C11" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D11" t="n">
-        <v>1010.86</v>
+        <v>1010.25</v>
       </c>
       <c r="E11" t="n">
         <v>17.5</v>
@@ -653,55 +653,55 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:23</t>
+          <t>2025-06-08 01:48:59</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>25.8</v>
+        <v>27.1</v>
       </c>
       <c r="C12" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D12" t="n">
-        <v>1010.87</v>
+        <v>1010.23</v>
       </c>
       <c r="E12" t="n">
-        <v>18.33</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:25</t>
+          <t>2025-06-08 01:49:01</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>25.8</v>
+        <v>27.1</v>
       </c>
       <c r="C13" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D13" t="n">
-        <v>1010.86</v>
+        <v>1010.24</v>
       </c>
       <c r="E13" t="n">
-        <v>17.5</v>
+        <v>18.33</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:27</t>
+          <t>2025-06-08 01:49:03</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>25.8</v>
+        <v>26.7</v>
       </c>
       <c r="C14" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D14" t="n">
-        <v>1010.82</v>
+        <v>1010.24</v>
       </c>
       <c r="E14" t="n">
         <v>16.67</v>
@@ -710,134 +710,134 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:29</t>
+          <t>2025-06-08 01:49:05</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>25.8</v>
+        <v>26.7</v>
       </c>
       <c r="C15" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D15" t="n">
-        <v>1010.91</v>
+        <v>1010.25</v>
       </c>
       <c r="E15" t="n">
-        <v>15.83</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:31</t>
+          <t>2025-06-08 01:49:07</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>25.8</v>
+        <v>26.7</v>
       </c>
       <c r="C16" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D16" t="n">
-        <v>1010.86</v>
+        <v>1010.28</v>
       </c>
       <c r="E16" t="n">
-        <v>95.83</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:33</t>
+          <t>2025-06-08 01:49:09</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>25.8</v>
+        <v>26.7</v>
       </c>
       <c r="C17" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D17" t="n">
-        <v>1010.84</v>
+        <v>1010.29</v>
       </c>
       <c r="E17" t="n">
-        <v>2319.17</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:35</t>
+          <t>2025-06-08 01:49:11</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>25.8</v>
+        <v>26.7</v>
       </c>
       <c r="C18" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D18" t="n">
-        <v>1010.89</v>
+        <v>1010.3</v>
       </c>
       <c r="E18" t="n">
-        <v>16.67</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:37</t>
+          <t>2025-06-08 01:49:13</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>25.8</v>
+        <v>26.7</v>
       </c>
       <c r="C19" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D19" t="n">
-        <v>1010.88</v>
+        <v>1010.32</v>
       </c>
       <c r="E19" t="n">
-        <v>854.17</v>
+        <v>350.83</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:39</t>
+          <t>2025-06-08 01:49:15</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>25.8</v>
+        <v>26.7</v>
       </c>
       <c r="C20" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D20" t="n">
-        <v>1010.87</v>
+        <v>1010.2</v>
       </c>
       <c r="E20" t="n">
-        <v>16.67</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-06-08 00:22:42</t>
+          <t>2025-06-08 01:49:17</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>25.8</v>
+        <v>26.7</v>
       </c>
       <c r="C21" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D21" t="n">
-        <v>1010.93</v>
+        <v>1010.3</v>
       </c>
       <c r="E21" t="n">
-        <v>17.5</v>
+        <v>18.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>